<commit_message>
Add presence for 24.02
</commit_message>
<xml_diff>
--- a/project-management/PresenceRegistration.xlsx
+++ b/project-management/PresenceRegistration.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4E186C-65D3-EB47-A942-2234C934C88F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22935" yWindow="-2880" windowWidth="30930" windowHeight="16440"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
   <si>
     <t>Presence Registration</t>
   </si>
@@ -59,12 +54,15 @@
   <si>
     <t>23.02</t>
   </si>
+  <si>
+    <t>24.02</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,30 +419,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -454,7 +452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -464,8 +462,11 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -478,8 +479,11 @@
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -492,8 +496,11 @@
       <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -506,8 +513,11 @@
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -520,8 +530,11 @@
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -534,9 +547,12 @@
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A4:A8">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:A8">
     <sortCondition ref="A4:A8"/>
   </sortState>
   <mergeCells count="1">
@@ -548,6 +564,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013B4C70294E7DF46A500E8356D81C0ED" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="810135ad89ca1cb6205c8a1e46be91bc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b665732-4bc3-4ee7-9255-d368a740d7d4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62720422b3b8217f62cc1c9896985efc" ns2:_="">
     <xsd:import namespace="2b665732-4bc3-4ee7-9255-d368a740d7d4"/>
@@ -679,22 +710,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB62B8CB-1E2C-422C-8279-767E7C924372}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2685570-0F8F-471B-99BB-A2FBDEDA81A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43220FB9-B464-42CA-85B5-5487719C7BCD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -710,21 +743,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2685570-0F8F-471B-99BB-A2FBDEDA81A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB62B8CB-1E2C-422C-8279-767E7C924372}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>